<commit_message>
Remove MyModel and create migration
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aris/Documents/1-RUHAH/1-website/ruhah-heroku/ruhah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216ACED6-B938-E043-9BA0-68D1CF911729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963FBA71-E9A5-ED44-976C-8534EBD7F3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{3E9E366C-3BC6-F04D-89F8-214C8ED2C3D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{3E9E366C-3BC6-F04D-89F8-214C8ED2C3D7}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3767" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3719" uniqueCount="873">
   <si>
     <t>occasion</t>
   </si>
@@ -2739,7 +2739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2808,25 +2808,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2856,12 +2843,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3296,7 +3277,7 @@
   </sheetPr>
   <dimension ref="A1:K336"/>
   <sheetViews>
-    <sheetView topLeftCell="A161" zoomScaleNormal="113" workbookViewId="0">
+    <sheetView zoomScaleNormal="113" workbookViewId="0">
       <selection activeCell="I182" sqref="I182"/>
     </sheetView>
   </sheetViews>
@@ -8714,8 +8695,8 @@
   </sheetPr>
   <dimension ref="A1:B1553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1537" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A1553" sqref="A1553"/>
+    <sheetView topLeftCell="A1539" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A1483" sqref="A1483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18961,7 +18942,7 @@
       </c>
     </row>
     <row r="1281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1281" s="5">
+      <c r="A1281" s="9">
         <v>70949159</v>
       </c>
       <c r="B1281" t="s">
@@ -19009,7 +18990,7 @@
       </c>
     </row>
     <row r="1287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1287">
+      <c r="A1287" s="8">
         <v>58006343</v>
       </c>
       <c r="B1287" t="s">
@@ -19113,7 +19094,7 @@
       </c>
     </row>
     <row r="1300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1300">
+      <c r="A1300" s="8">
         <v>14482479</v>
       </c>
       <c r="B1300" t="s">
@@ -19201,7 +19182,7 @@
       </c>
     </row>
     <row r="1311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1311">
+      <c r="A1311" s="8">
         <v>90764377</v>
       </c>
       <c r="B1311" t="s">
@@ -19273,7 +19254,7 @@
       </c>
     </row>
     <row r="1320" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1320">
+      <c r="A1320" s="8">
         <v>85033076</v>
       </c>
       <c r="B1320" t="s">
@@ -19329,7 +19310,7 @@
       </c>
     </row>
     <row r="1327" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1327">
+      <c r="A1327" s="8">
         <v>48941555</v>
       </c>
       <c r="B1327" t="s">
@@ -19385,7 +19366,7 @@
       </c>
     </row>
     <row r="1334" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1334">
+      <c r="A1334" s="8">
         <v>46779021</v>
       </c>
       <c r="B1334" t="s">
@@ -19465,7 +19446,7 @@
       </c>
     </row>
     <row r="1344" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1344">
+      <c r="A1344" s="8">
         <v>34117720</v>
       </c>
       <c r="B1344" t="s">
@@ -19561,7 +19542,7 @@
       </c>
     </row>
     <row r="1356" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1356">
+      <c r="A1356" s="8">
         <v>98819447</v>
       </c>
       <c r="B1356" t="s">
@@ -19625,7 +19606,7 @@
       </c>
     </row>
     <row r="1364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1364">
+      <c r="A1364" s="8">
         <v>40447580</v>
       </c>
       <c r="B1364" t="s">
@@ -19705,7 +19686,7 @@
       </c>
     </row>
     <row r="1374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1374">
+      <c r="A1374" s="8">
         <v>83063230</v>
       </c>
       <c r="B1374" t="s">
@@ -19833,7 +19814,7 @@
       </c>
     </row>
     <row r="1390" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1390" s="5">
+      <c r="A1390" s="9">
         <v>55379399</v>
       </c>
       <c r="B1390" t="s">
@@ -19921,7 +19902,7 @@
       </c>
     </row>
     <row r="1401" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1401">
+      <c r="A1401" s="8">
         <v>28373000</v>
       </c>
       <c r="B1401" t="s">
@@ -20009,7 +19990,7 @@
       </c>
     </row>
     <row r="1412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1412">
+      <c r="A1412" s="8">
         <v>67386615</v>
       </c>
       <c r="B1412" t="s">
@@ -20113,7 +20094,7 @@
       </c>
     </row>
     <row r="1425" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1425">
+      <c r="A1425" s="8">
         <v>82161484</v>
       </c>
       <c r="B1425" t="s">
@@ -20217,7 +20198,7 @@
       </c>
     </row>
     <row r="1438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1438">
+      <c r="A1438" s="8">
         <v>56909533</v>
       </c>
       <c r="B1438" t="s">
@@ -20313,7 +20294,7 @@
       </c>
     </row>
     <row r="1450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1450">
+      <c r="A1450" s="8">
         <v>26275839</v>
       </c>
       <c r="B1450" t="s">
@@ -20369,7 +20350,7 @@
       </c>
     </row>
     <row r="1457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1457">
+      <c r="A1457" s="8">
         <v>66175178</v>
       </c>
       <c r="B1457" t="s">
@@ -20417,7 +20398,7 @@
       </c>
     </row>
     <row r="1463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1463">
+      <c r="A1463" s="8">
         <v>77679075</v>
       </c>
       <c r="B1463" t="s">
@@ -20473,7 +20454,7 @@
       </c>
     </row>
     <row r="1470" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1470">
+      <c r="A1470" s="8">
         <v>88528528</v>
       </c>
       <c r="B1470" t="s">
@@ -20577,7 +20558,7 @@
       </c>
     </row>
     <row r="1483" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1483">
+      <c r="A1483" s="8">
         <v>39651001</v>
       </c>
       <c r="B1483" t="s">
@@ -20649,7 +20630,7 @@
       </c>
     </row>
     <row r="1492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1492">
+      <c r="A1492" s="8">
         <v>76239632</v>
       </c>
       <c r="B1492" t="s">
@@ -20721,7 +20702,7 @@
       </c>
     </row>
     <row r="1501" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1501">
+      <c r="A1501" s="8">
         <v>22121768</v>
       </c>
       <c r="B1501" t="s">
@@ -20809,7 +20790,7 @@
       </c>
     </row>
     <row r="1512" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1512">
+      <c r="A1512" s="8">
         <v>46980215</v>
       </c>
       <c r="B1512" t="s">
@@ -20889,7 +20870,7 @@
       </c>
     </row>
     <row r="1522" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1522">
+      <c r="A1522" s="8">
         <v>26210678</v>
       </c>
       <c r="B1522" t="s">
@@ -20961,7 +20942,7 @@
       </c>
     </row>
     <row r="1531" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1531">
+      <c r="A1531" s="8">
         <v>53292316</v>
       </c>
       <c r="B1531" t="s">
@@ -21033,7 +21014,7 @@
       </c>
     </row>
     <row r="1540" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1540">
+      <c r="A1540" s="8">
         <v>77853379</v>
       </c>
       <c r="B1540" t="s">
@@ -21097,7 +21078,7 @@
       </c>
     </row>
     <row r="1548" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1548">
+      <c r="A1548" s="8">
         <v>20129365</v>
       </c>
       <c r="B1548" t="s">
@@ -21160,7 +21141,7 @@
   </sheetPr>
   <dimension ref="A1:E552"/>
   <sheetViews>
-    <sheetView topLeftCell="A335" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="A378" zoomScale="113" workbookViewId="0">
       <selection activeCell="B353" sqref="B353"/>
     </sheetView>
   </sheetViews>
@@ -25925,443 +25906,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEA5CD6-C7E2-5C41-9C81-0E7439AD92B6}">
-  <dimension ref="D2:O26"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D2" s="17">
-        <v>58006343</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>809</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="19"/>
-    </row>
-    <row r="3" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D3" s="14">
-        <v>14482479</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>811</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="20"/>
-    </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D4" s="17">
-        <v>90764377</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>812</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18" t="s">
-        <v>416</v>
-      </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="19"/>
-    </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D5" s="15">
-        <v>85033076</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D6" s="17">
-        <v>48941555</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>814</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D7" s="15">
-        <v>46779021</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>817</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D8" s="17">
-        <v>34117720</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>821</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D9" s="15">
-        <v>98819447</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>824</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D10" s="17">
-        <v>40447580</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>825</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D11" s="15">
-        <v>83063230</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>830</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D12" s="17">
-        <v>55379399</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>831</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D13" s="15">
-        <v>28373000</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>836</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D14" s="17">
-        <v>67386615</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>838</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D15" s="15">
-        <v>82161484</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>839</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D16" s="17">
-        <v>56909533</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>843</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D17" s="15">
-        <v>26275839</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>844</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D18" s="17">
-        <v>66175178</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>847</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D19" s="15">
-        <v>77679075</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>848</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D20" s="17">
-        <v>88528528</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>864</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D21" s="15">
-        <v>39651001</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>852</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D22" s="17">
-        <v>76239632</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>856</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D23" s="15">
-        <v>22121768</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>857</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D24" s="17">
-        <v>46980215</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>859</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D25" s="15">
-        <v>26210678</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>860</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>